<commit_message>
modified code throughout to write and refer to file names by fiscal year. also made edits across code to begin doing error checks on the contracts data
</commit_message>
<xml_diff>
--- a/data/raw/2007_to_2017_NAICS.xlsx
+++ b/data/raw/2007_to_2017_NAICS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\britnee.pannell\Documents\GitHub_Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumeet.bedi\Documents\R\MEIS_Methodology\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC72E68E-067C-421A-B978-11CC4A8AC1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278A4B67-37CC-4E4F-B3AF-D34F134D241A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27450" yWindow="1335" windowWidth="15375" windowHeight="8325" xr2:uid="{0990EEED-D02E-4EA5-9855-C170BDE5023A}"/>
+    <workbookView xWindow="-16170" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{0990EEED-D02E-4EA5-9855-C170BDE5023A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,12 +394,12 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>315999</v>
       </c>
@@ -415,15 +415,15 @@
         <v>315990</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>316999</v>
       </c>
       <c r="B3">
-        <v>316990</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>316998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>315228</v>
       </c>
@@ -431,7 +431,7 @@
         <v>315220</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314912</v>
       </c>
@@ -439,7 +439,7 @@
         <v>314910</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>332212</v>
       </c>
@@ -447,7 +447,7 @@
         <v>332216</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>333313</v>
       </c>
@@ -455,7 +455,7 @@
         <v>333318</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>333319</v>
       </c>
@@ -463,7 +463,7 @@
         <v>333318</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>333518</v>
       </c>
@@ -471,7 +471,7 @@
         <v>333519</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>334119</v>
       </c>
@@ -479,7 +479,7 @@
         <v>334118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>334411</v>
       </c>
@@ -487,7 +487,7 @@
         <v>334419</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>339944</v>
       </c>
@@ -495,7 +495,7 @@
         <v>339940</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>443120</v>
       </c>

</xml_diff>